<commit_message>
added support and example for metastable isotopes
</commit_message>
<xml_diff>
--- a/tests/resources/libmanager/Activation libs.xlsx
+++ b/tests/resources/libmanager/Activation libs.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\d.laghi\Documents\GitHub\JADE\Configuration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATA\laghida\Documents\GitHub\F4Enix\tests\resources\libmanager\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4096B6D8-5CD7-4DB1-AC2E-9737F313796D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89ACB5CA-19FE-4617-8565-C5B130D7418B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0CD511ED-2E22-4867-A602-1EC939128E1A}"/>
   </bookViews>
@@ -749,12 +749,6 @@
     <t>Co57</t>
   </si>
   <si>
-    <t>Nb92</t>
-  </si>
-  <si>
-    <t>Ag110</t>
-  </si>
-  <si>
     <r>
       <t>(n,</t>
     </r>
@@ -942,6 +936,12 @@
   </si>
   <si>
     <t>(n,2n)+ (n,2n)*+(n,2n)**</t>
+  </si>
+  <si>
+    <t>Nb92m</t>
+  </si>
+  <si>
+    <t>Ag110m</t>
   </si>
 </sst>
 </file>
@@ -1276,7 +1276,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1292,9 +1292,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema di Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1332,7 +1332,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1438,7 +1438,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1580,7 +1580,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1590,17 +1590,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CBB7F4D4-921E-4A50-8836-A2E974A72224}">
   <dimension ref="A1:G101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J94" sqref="J94"/>
+    <sheetView tabSelected="1" topLeftCell="A81" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E108" sqref="E108"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="7" width="23.21875" style="8" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="8"/>
+    <col min="1" max="7" width="23.1796875" style="8" customWidth="1"/>
+    <col min="8" max="16384" width="8.90625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="25.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1623,7 +1623,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>9</v>
       </c>
@@ -1669,7 +1669,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="23"/>
       <c r="B4" s="4">
         <v>13</v>
@@ -1688,7 +1688,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
         <v>13</v>
       </c>
@@ -1711,7 +1711,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>15</v>
       </c>
@@ -1734,7 +1734,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="23"/>
       <c r="B7" s="4">
         <v>13</v>
@@ -1753,7 +1753,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
         <v>18</v>
       </c>
@@ -1776,7 +1776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
         <v>20</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -1822,7 +1822,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
         <v>29</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
         <v>31</v>
       </c>
@@ -1891,7 +1891,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="23"/>
       <c r="B14" s="4">
         <v>13</v>
@@ -1910,7 +1910,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
@@ -1956,7 +1956,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
         <v>37</v>
       </c>
@@ -1979,7 +1979,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="22" t="s">
         <v>40</v>
       </c>
@@ -2002,7 +2002,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="23"/>
       <c r="B19" s="4">
         <v>13</v>
@@ -2021,7 +2021,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="22" t="s">
         <v>42</v>
       </c>
@@ -2044,7 +2044,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="24"/>
       <c r="B21" s="6">
         <v>13</v>
@@ -2063,7 +2063,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="23"/>
       <c r="B22" s="4">
         <v>13</v>
@@ -2082,7 +2082,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="22" t="s">
         <v>44</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="24"/>
       <c r="B24" s="6">
         <v>13</v>
@@ -2124,7 +2124,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="23"/>
       <c r="B25" s="4">
         <v>13</v>
@@ -2143,7 +2143,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
         <v>45</v>
       </c>
@@ -2166,7 +2166,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
         <v>47</v>
       </c>
@@ -2189,7 +2189,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
         <v>49</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="3" t="s">
         <v>51</v>
       </c>
@@ -2235,7 +2235,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="22" t="s">
         <v>52</v>
       </c>
@@ -2258,7 +2258,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A31" s="23"/>
       <c r="B31" s="4">
         <v>12</v>
@@ -2277,7 +2277,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="22" t="s">
         <v>55</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="24"/>
       <c r="B33" s="6">
         <v>13</v>
@@ -2319,7 +2319,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="23"/>
       <c r="B34" s="4">
         <v>13</v>
@@ -2338,7 +2338,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="22" t="s">
         <v>57</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="24"/>
       <c r="B36" s="6">
         <v>13</v>
@@ -2380,7 +2380,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="23"/>
       <c r="B37" s="4">
         <v>13</v>
@@ -2399,7 +2399,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="22" t="s">
         <v>59</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="23"/>
       <c r="B39" s="4">
         <v>13</v>
@@ -2441,7 +2441,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="22" t="s">
         <v>60</v>
       </c>
@@ -2464,7 +2464,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="23"/>
       <c r="B41" s="4">
         <v>13</v>
@@ -2483,7 +2483,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="22" t="s">
         <v>62</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="24"/>
       <c r="B43" s="6">
         <v>13</v>
@@ -2525,7 +2525,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="24"/>
       <c r="B44" s="6">
         <v>13</v>
@@ -2544,7 +2544,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="23"/>
       <c r="B45" s="4">
         <v>13</v>
@@ -2563,7 +2563,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="22" t="s">
         <v>64</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="24"/>
       <c r="B47" s="6">
         <v>13</v>
@@ -2605,7 +2605,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="24"/>
       <c r="B48" s="6">
         <v>13</v>
@@ -2624,7 +2624,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="24"/>
       <c r="B49" s="6">
         <v>13</v>
@@ -2643,7 +2643,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="23"/>
       <c r="B50" s="4">
         <v>13</v>
@@ -2662,7 +2662,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="3" t="s">
         <v>67</v>
       </c>
@@ -2685,7 +2685,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="22" t="s">
         <v>70</v>
       </c>
@@ -2708,7 +2708,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="23"/>
       <c r="B53" s="4">
         <v>13</v>
@@ -2727,7 +2727,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="3" t="s">
         <v>72</v>
       </c>
@@ -2750,7 +2750,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="22" t="s">
         <v>73</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="23"/>
       <c r="B56" s="4">
         <v>13</v>
@@ -2792,7 +2792,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="3" t="s">
         <v>75</v>
       </c>
@@ -2815,7 +2815,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="3" t="s">
         <v>76</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="59" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="3" t="s">
         <v>78</v>
       </c>
@@ -2861,7 +2861,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="3" t="s">
         <v>79</v>
       </c>
@@ -2884,7 +2884,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="22" t="s">
         <v>81</v>
       </c>
@@ -2907,7 +2907,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="62" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A62" s="23"/>
       <c r="B62" s="4">
         <v>12</v>
@@ -2926,7 +2926,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="63" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="3" t="s">
         <v>85</v>
       </c>
@@ -2949,7 +2949,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" s="22" t="s">
         <v>86</v>
       </c>
@@ -2972,7 +2972,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="23"/>
       <c r="B65" s="4">
         <v>12</v>
@@ -2991,7 +2991,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" s="22" t="s">
         <v>88</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A67" s="23"/>
       <c r="B67" s="4">
         <v>13</v>
@@ -3033,7 +3033,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="5" t="s">
         <v>89</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="16" t="s">
         <v>91</v>
       </c>
@@ -3079,7 +3079,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="3" t="s">
         <v>93</v>
       </c>
@@ -3099,10 +3099,10 @@
         <v>94</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" s="22" t="s">
         <v>95</v>
       </c>
@@ -3122,10 +3122,10 @@
         <v>96</v>
       </c>
       <c r="G71" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72" s="23"/>
       <c r="B72" s="4">
         <v>13</v>
@@ -3144,7 +3144,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="5" t="s">
         <v>97</v>
       </c>
@@ -3167,7 +3167,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="74" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="16" t="s">
         <v>99</v>
       </c>
@@ -3190,7 +3190,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="5" t="s">
         <v>101</v>
       </c>
@@ -3213,7 +3213,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="16" t="s">
         <v>102</v>
       </c>
@@ -3233,10 +3233,10 @@
         <v>104</v>
       </c>
       <c r="G76" s="17" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A77" s="16" t="s">
         <v>105</v>
       </c>
@@ -3253,13 +3253,13 @@
         <v>102</v>
       </c>
       <c r="F77" s="18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G77" s="20" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A78" s="3" t="s">
         <v>107</v>
       </c>
@@ -3282,7 +3282,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A79" s="3" t="s">
         <v>109</v>
       </c>
@@ -3305,7 +3305,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="80" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A80" s="3" t="s">
         <v>111</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A81" s="3" t="s">
         <v>112</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" s="22" t="s">
         <v>114</v>
       </c>
@@ -3374,7 +3374,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="83" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A83" s="23"/>
       <c r="B83" s="4">
         <v>12</v>
@@ -3393,7 +3393,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="84" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="3" t="s">
         <v>116</v>
       </c>
@@ -3416,7 +3416,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" s="21" t="s">
         <v>118</v>
       </c>
@@ -3433,13 +3433,13 @@
         <v>102</v>
       </c>
       <c r="F85" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="G85" s="21" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="3" t="s">
         <v>120</v>
       </c>
@@ -3462,7 +3462,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A87" s="22" t="s">
         <v>122</v>
       </c>
@@ -3485,7 +3485,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="88" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="23"/>
       <c r="B88" s="4">
         <v>13</v>
@@ -3504,7 +3504,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" s="22" t="s">
         <v>124</v>
       </c>
@@ -3521,13 +3521,13 @@
         <v>28</v>
       </c>
       <c r="F89" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G89" s="6" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A90" s="23"/>
       <c r="B90" s="4">
         <v>13</v>
@@ -3540,13 +3540,13 @@
         <v>104</v>
       </c>
       <c r="F90" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="G90" s="4" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A91" s="3" t="s">
         <v>125</v>
       </c>
@@ -3569,7 +3569,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A92" s="3" t="s">
         <v>127</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" s="22" t="s">
         <v>129</v>
       </c>
@@ -3615,7 +3615,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="94" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A94" s="23"/>
       <c r="B94" s="4">
         <v>13</v>
@@ -3634,7 +3634,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="95" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A95" s="3" t="s">
         <v>132</v>
       </c>
@@ -3657,7 +3657,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A96" s="5" t="s">
         <v>134</v>
       </c>
@@ -3680,7 +3680,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="97" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A97" s="16" t="s">
         <v>135</v>
       </c>
@@ -3700,10 +3700,10 @@
         <v>38</v>
       </c>
       <c r="G97" s="17" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="98" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A98" s="16" t="s">
         <v>136</v>
       </c>
@@ -3720,13 +3720,13 @@
         <v>16</v>
       </c>
       <c r="F98" s="18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="G98" s="20" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="99" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A99" s="5" t="s">
         <v>138</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A100" s="16" t="s">
         <v>140</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A101" s="16" t="s">
         <v>142</v>
       </c>
@@ -3797,32 +3797,12 @@
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="A93:A94"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="A87:A88"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="A42:A45"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="C46:C50"/>
-    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="C6:C7"/>
+    <mergeCell ref="A13:A14"/>
+    <mergeCell ref="C13:C14"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="A30:A31"/>
@@ -3837,12 +3817,32 @@
     <mergeCell ref="A23:A25"/>
     <mergeCell ref="A32:A34"/>
     <mergeCell ref="C35:C37"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A13:A14"/>
-    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="A42:A45"/>
+    <mergeCell ref="A46:A50"/>
+    <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="C46:C50"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="C52:C53"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="A40:A41"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="A93:A94"/>
+    <mergeCell ref="C93:C94"/>
+    <mergeCell ref="A82:A83"/>
+    <mergeCell ref="C82:C83"/>
+    <mergeCell ref="A87:A88"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="C71:C72"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3854,16 +3854,16 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="16.33203125" style="8" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="8"/>
+    <col min="1" max="5" width="16.36328125" style="8" customWidth="1"/>
+    <col min="6" max="16384" width="8.90625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -3880,7 +3880,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="11" t="s">
         <v>146</v>
       </c>
@@ -3897,7 +3897,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="11" t="s">
         <v>4</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
@@ -3925,13 +3925,13 @@
         <v>102</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="11" t="s">
         <v>18</v>
       </c>
@@ -3942,13 +3942,13 @@
         <v>107</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="11" t="s">
         <v>49</v>
       </c>
@@ -3959,13 +3959,13 @@
         <v>102</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="11" t="s">
         <v>51</v>
       </c>
@@ -3982,7 +3982,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A8" s="25" t="s">
         <v>52</v>
       </c>
@@ -3999,7 +3999,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="27"/>
       <c r="B9" s="12">
         <v>13</v>
@@ -4008,13 +4008,13 @@
         <v>102</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E9" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A10" s="25" t="s">
         <v>55</v>
       </c>
@@ -4031,7 +4031,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="27"/>
       <c r="B11" s="12">
         <v>13</v>
@@ -4040,13 +4040,13 @@
         <v>107</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E11" s="12" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A12" s="25" t="s">
         <v>57</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A13" s="27"/>
       <c r="B13" s="12">
         <v>13</v>
@@ -4078,7 +4078,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="25" t="s">
         <v>59</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A15" s="27"/>
       <c r="B15" s="12">
         <v>13</v>
@@ -4110,7 +4110,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A16" s="25" t="s">
         <v>60</v>
       </c>
@@ -4121,13 +4121,13 @@
         <v>102</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A17" s="27"/>
       <c r="B17" s="12">
         <v>13</v>
@@ -4142,7 +4142,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A18" s="25" t="s">
         <v>62</v>
       </c>
@@ -4159,7 +4159,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A19" s="26"/>
       <c r="B19" s="13">
         <v>13</v>
@@ -4168,13 +4168,13 @@
         <v>102</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E19" s="13" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A20" s="26"/>
       <c r="B20" s="13">
         <v>13</v>
@@ -4189,7 +4189,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="27"/>
       <c r="B21" s="12">
         <v>13</v>
@@ -4198,13 +4198,13 @@
         <v>107</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E21" s="12" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="11" t="s">
         <v>64</v>
       </c>
@@ -4221,7 +4221,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="11" t="s">
         <v>67</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A24" s="25" t="s">
         <v>70</v>
       </c>
@@ -4255,7 +4255,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A25" s="27"/>
       <c r="B25" s="12">
         <v>13</v>
@@ -4270,7 +4270,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="11" t="s">
         <v>72</v>
       </c>
@@ -4281,13 +4281,13 @@
         <v>107</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E26" s="12" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="25" t="s">
         <v>73</v>
       </c>
@@ -4304,7 +4304,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="26"/>
       <c r="B28" s="13">
         <v>13</v>
@@ -4313,13 +4313,13 @@
         <v>102</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E28" s="13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="27"/>
       <c r="B29" s="12">
         <v>13</v>
@@ -4328,13 +4328,13 @@
         <v>107</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A30" s="25" t="s">
         <v>75</v>
       </c>
@@ -4351,7 +4351,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="26"/>
       <c r="B31" s="13">
         <v>13</v>
@@ -4360,13 +4360,13 @@
         <v>102</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E31" s="13" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="27"/>
       <c r="B32" s="12">
         <v>13</v>
@@ -4381,7 +4381,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="11" t="s">
         <v>118</v>
       </c>
@@ -4392,13 +4392,13 @@
         <v>102</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="11" t="s">
         <v>122</v>
       </c>
@@ -4415,7 +4415,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="11" t="s">
         <v>127</v>
       </c>
@@ -4426,7 +4426,7 @@
         <v>102</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E35" s="12" t="s">
         <v>128</v>

</xml_diff>